<commit_message>
add listing  changes  and  api  changes
add listing  changes  and  api  changes
</commit_message>
<xml_diff>
--- a/assets/subcategoryimportfiles/Electronicheadphone.xlsx
+++ b/assets/subcategoryimportfiles/Electronicheadphone.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>sno</t>
   </si>
@@ -121,9 +121,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>dress</t>
-  </si>
-  <si>
     <t>dress_code</t>
   </si>
   <si>
@@ -149,6 +146,21 @@
   </si>
   <si>
     <t>In Sales Package</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>useage</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Microphone</t>
+  </si>
+  <si>
+    <t>sonyhead</t>
   </si>
 </sst>
 </file>
@@ -573,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -598,11 +610,11 @@
     <col min="18" max="18" width="33.28515625" customWidth="1"/>
     <col min="19" max="19" width="48" customWidth="1"/>
     <col min="20" max="20" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="27" width="48.28515625" customWidth="1"/>
-    <col min="28" max="29" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="31" width="48.28515625" customWidth="1"/>
+    <col min="32" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="5" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:39" s="5" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -663,58 +675,70 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AC1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AD1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AE1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:39">
       <c r="A2" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C2" s="7">
         <v>5000</v>
@@ -742,43 +766,55 @@
         <v>31</v>
       </c>
       <c r="S2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="Y2" t="s">
         <v>36</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Z2" t="s">
         <v>37</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AA2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" t="s">
         <v>38</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AC2" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AD2" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AE2" t="s">
         <v>41</v>
       </c>
-      <c r="AA2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
       <c r="AF2" s="12"/>
       <c r="AG2" s="12"/>
       <c r="AH2" s="12"/>
       <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AB1:XFD1 A1:N1 Q1:T1">
+  <conditionalFormatting sqref="AF1:XFD1 A1:N1 Q1:U1">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -790,7 +826,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ1:XFD1 H1:N1 A1">
+  <conditionalFormatting sqref="AN1:XFD1 H1:N1 A1">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
seller in add listing  changes purpose
seller in add listing  changes purpose
</commit_message>
<xml_diff>
--- a/assets/subcategoryimportfiles/Electronicheadphone.xlsx
+++ b/assets/subcategoryimportfiles/Electronicheadphone.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>sno</t>
   </si>
@@ -161,6 +161,30 @@
   </si>
   <si>
     <t>sonyhead</t>
+  </si>
+  <si>
+    <t>gh</t>
+  </si>
+  <si>
+    <t>hfgh</t>
+  </si>
+  <si>
+    <t>fghfgh</t>
+  </si>
+  <si>
+    <t>fhdfg</t>
+  </si>
+  <si>
+    <t>fgd</t>
+  </si>
+  <si>
+    <t>fgh</t>
+  </si>
+  <si>
+    <t>hfdgh</t>
+  </si>
+  <si>
+    <t>fg</t>
   </si>
 </sst>
 </file>
@@ -587,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -804,14 +828,30 @@
       <c r="AE2" t="s">
         <v>41</v>
       </c>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="12"/>
+      <c r="AF2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM2" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="AF1:XFD1 A1:N1 Q1:U1">

</xml_diff>